<commit_message>
update verification charts (consistency and continuity)
</commit_message>
<xml_diff>
--- a/Analysis/verification/consistency_test/mean_waiting_time/bosses/10_repetitions/test_with_1-2-15.xlsx
+++ b/Analysis/verification/consistency_test/mean_waiting_time/bosses/10_repetitions/test_with_1-2-15.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -110,11 +110,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -137,9 +138,15 @@
       <color rgb="FF2A6099"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="13"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -278,7 +285,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -298,7 +305,7 @@
               <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
                 <a:latin typeface="Arial"/>
               </a:rPr>
-              <a:t>Bosses Mean Waiting Time E[W]</a:t>
+              <a:t>Consistency Test - Bosses Mean Waiting Time E[W]</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -340,39 +347,7 @@
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:invertIfNegative val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
           <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:txPr>
-                <a:bodyPr/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                      <a:latin typeface="Arial"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator> </c:separator>
-            </c:dLbl>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -384,6 +359,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -465,39 +441,7 @@
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:invertIfNegative val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
           <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:txPr>
-                <a:bodyPr/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                      <a:latin typeface="Arial"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator> </c:separator>
-            </c:dLbl>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -509,6 +453,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -556,7 +501,7 @@
           </c:errBars>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$17:$J$17</c:f>
+              <c:f>Sheet1!$J$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -590,7 +535,40 @@
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -602,6 +580,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -649,7 +628,7 @@
           </c:errBars>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$33:$J$33</c:f>
+              <c:f>Sheet1!$J$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -662,11 +641,11 @@
         </c:ser>
         <c:gapWidth val="400"/>
         <c:overlap val="-100"/>
-        <c:axId val="18408382"/>
-        <c:axId val="3973832"/>
+        <c:axId val="10438222"/>
+        <c:axId val="21438600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="18408382"/>
+        <c:axId val="10438222"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -722,7 +701,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="3973832"/>
+        <c:crossAx val="21438600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -730,7 +709,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="3973832"/>
+        <c:axId val="21438600"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -762,7 +741,7 @@
                   <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
-                  <a:t>Mean Waiting Time E[W] [seconds]</a:t>
+                  <a:t>Waiting Time E[W] [s]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -775,7 +754,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -797,10 +776,9 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="18408382"/>
+        <c:crossAx val="10438222"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="1"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -813,16 +791,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.201233365790328"/>
-          <c:y val="0.901571621014818"/>
-          <c:w val="0.64367629557503"/>
-          <c:h val="0.0536147283340817"/>
-        </c:manualLayout>
-      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -849,7 +817,7 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
@@ -861,15 +829,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>789480</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>487800</xdr:rowOff>
+      <xdr:colOff>781560</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>57240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>129240</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>64800</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>514080</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>125640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -877,8 +845,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="16231320" y="487800"/>
-        <a:ext cx="6654960" cy="4008600"/>
+        <a:off x="16243560" y="587160"/>
+        <a:ext cx="6255360" cy="4132440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -898,11 +866,11 @@
   </sheetPr>
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="X13" activeCellId="0" sqref="X13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M21" activeCellId="0" sqref="M21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.09"/>

</xml_diff>